<commit_message>
changed xl to change hash
</commit_message>
<xml_diff>
--- a/data_examples/MasterDataBook v2.xlsx
+++ b/data_examples/MasterDataBook v2.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Current Assets</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Stay Below</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -554,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1127,6 +1130,11 @@
       <c r="I34">
         <f t="shared" si="14"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
next up date to change hash
</commit_message>
<xml_diff>
--- a/data_examples/MasterDataBook v2.xlsx
+++ b/data_examples/MasterDataBook v2.xlsx
@@ -126,7 +126,7 @@
     <t>Stay Below</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -559,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
next up date to change hash 2
</commit_message>
<xml_diff>
--- a/data_examples/MasterDataBook v2.xlsx
+++ b/data_examples/MasterDataBook v2.xlsx
@@ -126,7 +126,7 @@
     <t>Stay Below</t>
   </si>
   <si>
-    <t>.</t>
+    <t>..</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>